<commit_message>
Updated ControlRouteSuitability and FilterInformationFromERTMSTrackside sheets.
Updated ControlRouteSuitability interfaces diagram.
</commit_message>
<xml_diff>
--- a/System Analysis/WorkingRepository/Group1/ControlRouteSuitability.xlsx
+++ b/System Analysis/WorkingRepository/Group1/ControlRouteSuitability.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,12 @@
   <definedNames>
     <definedName name="__DdeLink__1724_1104613906" localSheetId="2">Requirements!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="158">
   <si>
     <t>Authors:</t>
   </si>
@@ -286,9 +286,6 @@
     <t>SA-6</t>
   </si>
   <si>
-    <t>The DMI shall inform the driver about all unsuitabilities from ListOfUnsuitabilities.</t>
-  </si>
-  <si>
     <t>DMI</t>
   </si>
   <si>
@@ -298,9 +295,6 @@
     <t>The Kernel shall send route suitability parts of TrainData through Packet11 to the RBC.</t>
   </si>
   <si>
-    <t>Kernel but other function</t>
-  </si>
-  <si>
     <t>SRS-3.12.2.9.1</t>
   </si>
   <si>
@@ -310,9 +304,6 @@
     <t>SA-1</t>
   </si>
   <si>
-    <t>The Kernel shall compare RouteSuitabilityData with TrainData, and build the list of unsuitabilities (if any).</t>
-  </si>
-  <si>
     <t>SRS-3.12.2.3</t>
   </si>
   <si>
@@ -322,30 +313,18 @@
     <t>SA-2</t>
   </si>
   <si>
-    <t>a) The Kernel shall add an unsuitability to the list of unsuitabilities if TrainData.M_LOADINGGAUGE is not in the list indicated by RouteSuitabilityData.M_LINEGAUGE.</t>
-  </si>
-  <si>
     <t>SRS-3.12.2.3, SRS-7.4.2.21</t>
   </si>
   <si>
     <t>SA-3</t>
   </si>
   <si>
-    <t>b) The Kernel shall add an unsuitability to the list of unsuitabilities if the traction system indicated by RouteSuitabilityData.M_VOLTAGE and RouteSuitabilityData.NID_CTRACTION is not in TrainData.ListOfAcceptedTractionSystems</t>
-  </si>
-  <si>
     <t>SA-4</t>
   </si>
   <si>
-    <t>c) The Kernel shall add an unsuitability to the list of unsuitabilities if TrainData.AxleLoadCategory &gt; RouteSuitabilityData.M_AXLELOADCAT</t>
-  </si>
-  <si>
     <t>SA-5</t>
   </si>
   <si>
-    <t>If ListOfUnsuitabilities contains at least one unsuitability, the Kernel shall set ClosestUnsuitabilityLocation with the closest location corresponding to the unsuitabilities of the list, and replace both EndOfAuthority and SupervisedLocation with ClosestUnsuitabilityLocation, and set ReleaseSpeed to a NO_RELEASE_SPEED value.</t>
-  </si>
-  <si>
     <t>SRS-3.12.2.4</t>
   </si>
   <si>
@@ -373,24 +352,12 @@
     <t>Subset-23, Subset-26-3</t>
   </si>
   <si>
-    <t>Packet70</t>
-  </si>
-  <si>
     <t xml:space="preserve">SRS-3.12.2.1, </t>
   </si>
   <si>
-    <t>TrainData</t>
-  </si>
-  <si>
-    <t>Defined set of data which gives information about the train. Data that characterises a train and which is required by ERTMS/ETCS in order to supervise a train movement.</t>
-  </si>
-  <si>
     <t>SA-1, SA-2, SA-3, SA-4</t>
   </si>
   <si>
-    <t>ListOfUnsuitabilities</t>
-  </si>
-  <si>
     <t>List of route suitabilities where incompatibilities occur for this train.</t>
   </si>
   <si>
@@ -400,9 +367,6 @@
     <t>ClosestUnsuitabilityLocation</t>
   </si>
   <si>
-    <t>The closest location (from the train location) corresponding to the unsuitabilities of ListOfUnsuitabilities</t>
-  </si>
-  <si>
     <t>EndOfAuthority</t>
   </si>
   <si>
@@ -425,14 +389,6 @@
   </si>
   <si>
     <t>ControlRouteSuitability</t>
-  </si>
-  <si>
-    <t>* compares RouteSuitabilityData (Packet70) from trackside  with TrainData to determine the list of unsuitabilities
-* replaces movement authority data with the closest unsuitability location if there is some</t>
-  </si>
-  <si>
-    <t>RouteSuitabilityData (Packet70)
-TrainData</t>
   </si>
   <si>
     <t>SA-1, 
@@ -598,8 +554,47 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Location to shorten track information (not represented on the figure) represents a location where MA, track description and linking information must be deleted (see 026-A3.4 Handling of Accepted and Stored Information in specific Situations).</t>
+      <t>« Perform train protection » supervises the new EOA provided by the closest unsuitability, if any.</t>
     </r>
+  </si>
+  <si>
+    <t>* « Interface with DMI » sends unsuitability information to DMI, if any.</t>
+  </si>
+  <si>
+    <t>* Initially, there is no route suitability restriction [3.12.2.10]</t>
+  </si>
+  <si>
+    <t>* When the function receives new route suitability data [3.12.2.2], the new identified route unsuitability information of any type (loading gauge or traction system or axle load) shall replace all stored route unsuitability information of the same type.</t>
+  </si>
+  <si>
+    <t>* The function shall delete the stored route suitability data from a given location, if required by another function (location to shorten track information [A3.4])</t>
+  </si>
+  <si>
+    <t>* The function shall delete the stored route suitability data when it detects a change of mode according to the conditions defined in [4.10].</t>
+  </si>
+  <si>
+    <t>* The function shall check route suitability data in FS, LS and OS mode [4.5.2]</t>
+  </si>
+  <si>
+    <t>* The function shall check if the train is suitable with respect to the received route suitability data as follows [3.12.2.3] :</t>
+  </si>
+  <si>
+    <t>* In case of unsuitability [3.12.2.4]:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   c. there is a route unsuitability if the list of traction systems supported by the train does not include the traction system supported by the track (M_VOLTAGE and NID_CTRACTION)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    b. there is a route unsuitability if the axle load category of the train is above the permitted one received from trackside, (M_AXLELOADCAT).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a. there is a route unsuitability if the loading gauge of the train M_LOADINGGAUGE is not in the list of loading gauges supported by the track (M_LINEGAUGE).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   a. The driver shall be informed by a text message (one per type of unsuitability) about all new route unsuitabilities (corresponding to the current train data) at their reception. This displayed information shall be re-evaluated at each reception of new route unsuitability information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    b. The location where the closest route unsuitability begins shall be identified (closest unsuitability location) as EOA/SVL to allow train supervision functions to avoid the entry of the train in the unsuitable area.</t>
   </si>
   <si>
     <r>
@@ -621,53 +616,94 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>« Perform train protection » supervises the new EOA provided by the closest unsuitability, if any.</t>
+      <t>Location to shorten track information represents a location where MA, track description and linking information must be deleted (see 026-A3.4 Handling of Accepted and Stored Information in specific Situations).</t>
     </r>
   </si>
   <si>
-    <t>* « Interface with DMI » sends unsuitability information to DMI, if any.</t>
-  </si>
-  <si>
-    <t>* Initially, there is no route suitability restriction [3.12.2.10]</t>
-  </si>
-  <si>
-    <t>* When the function receives new route suitability data [3.12.2.2], the new identified route unsuitability information of any type (loading gauge or traction system or axle load) shall replace all stored route unsuitability information of the same type.</t>
-  </si>
-  <si>
-    <t>* The function shall delete the stored route suitability data from a given location, if required by another function (location to shorten track information [A3.4])</t>
-  </si>
-  <si>
-    <t>* The function shall delete the stored route suitability data when it detects a change of mode according to the conditions defined in [4.10].</t>
-  </si>
-  <si>
-    <t>* The function shall check route suitability data in FS, LS and OS mode [4.5.2]</t>
-  </si>
-  <si>
-    <t>* The function shall check if the train is suitable with respect to the received route suitability data as follows [3.12.2.3] :</t>
-  </si>
-  <si>
-    <t>* In case of unsuitability [3.12.2.4]:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   c. there is a route unsuitability if the list of traction systems supported by the train does not include the traction system supported by the track (M_VOLTAGE and NID_CTRACTION)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    b. there is a route unsuitability if the axle load category of the train is above the permitted one received from trackside, (M_AXLELOADCAT).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    a. there is a route unsuitability if the loading gauge of the train M_LOADINGGAUGE is not in the list of loading gauges supported by the track (M_LINEGAUGE).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   a. The driver shall be informed by a text message (one per type of unsuitability) about all new route unsuitabilities (corresponding to the current train data) at their reception. This displayed information shall be re-evaluated at each reception of new route unsuitability information.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    b. The location where the closest route unsuitability begins shall be identified (closest unsuitability location) as EOA/SVL to allow train supervision functions to avoid the entry of the train in the unsuitable area.</t>
+    <t>* Initially, there is no route suitability restriction [3.12.2.10]
+* When the function receives new route suitability data [3.12.2.2], the new identified route unsuitability information of any type (loading gauge or traction system or axle load) shall replace all stored route unsuitability information of the same type.
+* The function shall delete the stored route suitability data from a given location, if required by another function (location to shorten track information [A3.4])
+* The function shall delete the stored route suitability data when it detects a change of mode according to the conditions defined in [4.10].
+* The function shall check route suitability data in FS, LS and OS mode [4.5.2]
+* The function shall check if the train is suitable with respect to the received route suitability data as follows [3.12.2.3] :
+    a. there is a route unsuitability if the loading gauge of the train M_LOADINGGAUGE is not in the list of loading gauges supported by the track (M_LINEGAUGE).
+    b. there is a route unsuitability if the axle load category of the train is above the permitted one received from trackside, (M_AXLELOADCAT).
+    c. there is a route unsuitability if the list of traction systems supported by the train does not include the traction system supported by the track (M_VOLTAGE and NID_CTRACTION)
+* In case of unsuitability [3.12.2.4]:
+    a. The driver shall be informed by a text message (one per type of unsuitability) about all new route unsuitabilities (corresponding to the current train data) at their reception. This displayed information shall be re-evaluated at each reception of new route unsuitability information.
+    b. The location where the closest route unsuitability begins shall be identified (closest unsuitability location) as EOA/SVL to allow train supervision functions to avoid the entry of the train in the unsuitable area.</t>
+  </si>
+  <si>
+    <t>Mode, TrainSuitabilityData, RouteSuitabilityData, LocationToShortenTrack</t>
+  </si>
+  <si>
+    <t>Unsuitabilities, ClosestUnsuitabilityLocation</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>T_Mode</t>
+  </si>
+  <si>
+    <t>T_RouteSuitabilityData</t>
+  </si>
+  <si>
+    <t>TrainSuitabilityData</t>
+  </si>
+  <si>
+    <t>Subset of TrainData which gives information about the train suitability (gauge, axle load category, traction system).</t>
+  </si>
+  <si>
+    <t>T_TrainSuitabilityData</t>
+  </si>
+  <si>
+    <t>Unsuitabilities</t>
+  </si>
+  <si>
+    <t>List of T_Unsuitability</t>
+  </si>
+  <si>
+    <t>The closest unsuitability location (from the train location).</t>
+  </si>
+  <si>
+    <t>T_Location</t>
+  </si>
+  <si>
+    <t>T_Speed</t>
+  </si>
+  <si>
+    <t>T_Packet</t>
+  </si>
+  <si>
+    <t>The DMI shall inform the driver about all unsuitabilities from Unsuitabilities.</t>
+  </si>
+  <si>
+    <t>Kernel (but other function)</t>
+  </si>
+  <si>
+    <t>a) The Kernel shall add an unsuitability to the list of unsuitabilities if TrainSuitabilityData.LoadingGauge is not in the list indicated by RouteSuitabilityData.LineGauges.</t>
+  </si>
+  <si>
+    <t>b) The Kernel shall add an unsuitability to the list Unsuitabilities if the RouteSuitabilityData.TractionSystem is not in TrainSuitabilityData.TractionSystems</t>
+  </si>
+  <si>
+    <t>c) The Kernel shall add an unsuitability to the list Unsuitabilities if TrainSuitabilityData.AxleLoadCategory &gt; RouteSuitabilityData.MaxAxleLoadCategory</t>
+  </si>
+  <si>
+    <t>The Kernel shall compare RouteSuitabilityData with TrainSuitabilityData, and build the list of unsuitabilities (if any).</t>
+  </si>
+  <si>
+    <t>If Unsuitabilities contains at least one unsuitability, the Kernel shall set ClosestUnsuitabilityLocation with the closest location corresponding to the unsuitabilities of the list, and take this location into account when computing EndOfAuthority, SupervisedLocation, and ReleaseSpeed.</t>
+  </si>
+  <si>
+    <t>20/11/2013 - v7 - Updated functions, requirements and variables regarding the SysML model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="18">
     <font>
       <sz val="11"/>
@@ -1037,6 +1073,22 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1052,6 +1104,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1076,25 +1131,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1115,14 +1151,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>142873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>173335</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>625429</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>3328587</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1132,22 +1168,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="13182601"/>
-          <a:ext cx="5305425" cy="4107159"/>
+          <a:off x="0" y="12468223"/>
+          <a:ext cx="6721429" cy="3185714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1155,7 +1184,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1190,10 +1219,10 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1291,7 +1320,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1326,7 +1354,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1502,25 +1529,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:G76"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="1"/>
@@ -1539,7 +1566,7 @@
     <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:7" s="43" customFormat="1" ht="15.75">
+    <row r="7" spans="1:7" s="29" customFormat="1" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1598,519 +1625,524 @@
     </row>
     <row r="20" spans="1:7" ht="15.75">
       <c r="A20" s="17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="18.75">
-      <c r="A22" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75">
+      <c r="A21" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="16.5">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="18.75">
+      <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75">
-      <c r="A24" s="17" t="s">
-        <v>47</v>
-      </c>
+    <row r="24" spans="1:7" ht="18.75">
+      <c r="A24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="15.75">
       <c r="A25" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75">
+      <c r="A26" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75">
-      <c r="A26" s="17"/>
-    </row>
-    <row r="27" spans="1:7" ht="18.75">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:7" ht="15.75">
+      <c r="A27" s="17"/>
     </row>
     <row r="28" spans="1:7" ht="18.75">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.75">
+      <c r="A29" s="18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A29" s="24" t="s">
+    <row r="30" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A30" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-    </row>
-    <row r="30" spans="1:7" ht="21.75" customHeight="1">
-      <c r="A30" s="27" t="s">
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+    </row>
+    <row r="31" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A31" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-    </row>
-    <row r="31" spans="1:7" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+    </row>
+    <row r="32" spans="1:7" ht="40.5" customHeight="1">
+      <c r="A32" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-    </row>
-    <row r="32" spans="1:7" ht="53.25" customHeight="1">
-      <c r="A32" s="28" t="s">
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+    </row>
+    <row r="33" spans="1:7" ht="53.25" customHeight="1">
+      <c r="A33" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75">
-      <c r="A33" s="17"/>
-    </row>
-    <row r="34" spans="1:7" ht="60.75" customHeight="1">
-      <c r="A34" s="24" t="s">
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75">
+      <c r="A34" s="17"/>
+    </row>
+    <row r="35" spans="1:7" ht="60.75" customHeight="1">
+      <c r="A35" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75">
-      <c r="A35" s="17"/>
-    </row>
-    <row r="36" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A36" s="24" t="s">
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75">
+      <c r="A36" s="17"/>
+    </row>
+    <row r="37" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A37" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-    </row>
-    <row r="37" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A37" s="25" t="s">
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+    </row>
+    <row r="38" spans="1:7" ht="35.25" customHeight="1">
+      <c r="A38" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-    </row>
-    <row r="38" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A38" s="24" t="s">
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+    </row>
+    <row r="39" spans="1:7" ht="28.5" customHeight="1">
+      <c r="A39" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-    </row>
-    <row r="39" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A39" s="24" t="s">
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+    </row>
+    <row r="40" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A40" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-    </row>
-    <row r="40" spans="1:7" ht="15.75">
-      <c r="A40" s="17"/>
-    </row>
-    <row r="41" spans="1:7" ht="18.75">
-      <c r="A41" s="18" t="s">
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" spans="1:7" ht="15.75">
+      <c r="A41" s="17"/>
+    </row>
+    <row r="42" spans="1:7" ht="18.75">
+      <c r="A42" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75">
+      <c r="A43" s="27" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="48" customHeight="1">
+      <c r="A44" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.75">
+      <c r="A45" s="17"/>
+    </row>
+    <row r="46" spans="1:7" ht="279.75" customHeight="1">
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.75">
+      <c r="A52" s="17"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75">
+      <c r="A53" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+    </row>
+    <row r="54" spans="1:7" ht="66" customHeight="1">
+      <c r="A54" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+    </row>
+    <row r="55" spans="1:7" ht="46.5" customHeight="1">
+      <c r="A55" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+    </row>
+    <row r="56" spans="1:7" ht="52.5" customHeight="1">
+      <c r="A56" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+    </row>
+    <row r="57" spans="1:7" ht="51" customHeight="1">
+      <c r="A57" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="31"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="31"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75">
+      <c r="A58" s="31"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
+    </row>
+    <row r="59" spans="1:7" ht="123.75" customHeight="1">
+      <c r="A59" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.75">
+      <c r="A60" s="31"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+    </row>
+    <row r="61" spans="1:7" ht="42" customHeight="1">
+      <c r="A61" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" s="31"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="31"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75">
+      <c r="A62" s="31"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75">
+      <c r="A63" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="31"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.75">
+      <c r="A64" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+    </row>
+    <row r="65" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A65" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+    </row>
+    <row r="66" spans="1:7" ht="15.75">
+      <c r="A66" s="28"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.75">
+      <c r="A67" s="27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A68" s="31" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75">
-      <c r="A42" s="40" t="s">
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+    </row>
+    <row r="69" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A69" s="31" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="48" customHeight="1">
-      <c r="A43" s="24" t="s">
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="31"/>
+    </row>
+    <row r="70" spans="1:7" ht="40.5" customHeight="1">
+      <c r="A70" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-    </row>
-    <row r="44" spans="1:7" ht="15.75">
-      <c r="A44" s="17"/>
-    </row>
-    <row r="45" spans="1:7" ht="279.75" customHeight="1">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="42"/>
-      <c r="E45" s="42"/>
-    </row>
-    <row r="51" spans="1:7" ht="15.75">
-      <c r="A51" s="17"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75">
-      <c r="A52" s="25" t="s">
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="31"/>
+    </row>
+    <row r="71" spans="1:7" ht="36" customHeight="1">
+      <c r="A71" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-    </row>
-    <row r="53" spans="1:7" ht="66" customHeight="1">
-      <c r="A53" s="25" t="s">
+      <c r="B71" s="31"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="31"/>
+      <c r="G71" s="31"/>
+    </row>
+    <row r="72" spans="1:7" ht="20.25" customHeight="1">
+      <c r="A72" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B72" s="31"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="31"/>
+    </row>
+    <row r="73" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A73" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" s="31"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="31"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+    </row>
+    <row r="74" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A74" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-    </row>
-    <row r="54" spans="1:7" ht="46.5" customHeight="1">
-      <c r="A54" s="25" t="s">
+      <c r="B74" s="31"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+    </row>
+    <row r="75" spans="1:7" ht="46.5" customHeight="1">
+      <c r="A75" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="B75" s="31"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+    </row>
+    <row r="76" spans="1:7" ht="47.25" customHeight="1">
+      <c r="A76" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B76" s="31"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
+    </row>
+    <row r="77" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A77" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="B77" s="31"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+    </row>
+    <row r="78" spans="1:7" ht="69.75" customHeight="1">
+      <c r="A78" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-    </row>
-    <row r="55" spans="1:7" ht="52.5" customHeight="1">
-      <c r="A55" s="25" t="s">
+      <c r="B78" s="31"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+    </row>
+    <row r="79" spans="1:7" ht="48" customHeight="1">
+      <c r="A79" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="25"/>
-    </row>
-    <row r="56" spans="1:7" ht="51" customHeight="1">
-      <c r="A56" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-    </row>
-    <row r="57" spans="1:7" ht="15.75">
-      <c r="A57" s="25"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25"/>
-    </row>
-    <row r="58" spans="1:7" ht="123.75" customHeight="1">
-      <c r="A58" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75">
-      <c r="A59" s="25"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="25"/>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25"/>
-    </row>
-    <row r="60" spans="1:7" ht="42" customHeight="1">
-      <c r="A60" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
-      <c r="D60" s="25"/>
-      <c r="E60" s="25"/>
-      <c r="F60" s="25"/>
-      <c r="G60" s="25"/>
-    </row>
-    <row r="61" spans="1:7" ht="15.75">
-      <c r="A61" s="25"/>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="25"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75">
-      <c r="A62" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="25"/>
-      <c r="G62" s="25"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75">
-      <c r="A63" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
-    </row>
-    <row r="64" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A64" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="25"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="25"/>
-    </row>
-    <row r="65" spans="1:7" ht="15.75">
-      <c r="A65" s="41"/>
-    </row>
-    <row r="66" spans="1:7" ht="15.75">
-      <c r="A66" s="40" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A67" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25"/>
-    </row>
-    <row r="68" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A68" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-      <c r="G68" s="25"/>
-    </row>
-    <row r="69" spans="1:7" ht="40.5" customHeight="1">
-      <c r="A69" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="25"/>
-      <c r="F69" s="25"/>
-      <c r="G69" s="25"/>
-    </row>
-    <row r="70" spans="1:7" ht="36" customHeight="1">
-      <c r="A70" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="E70" s="25"/>
-      <c r="F70" s="25"/>
-      <c r="G70" s="25"/>
-    </row>
-    <row r="71" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A71" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
-      <c r="G71" s="25"/>
-    </row>
-    <row r="72" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A72" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
-      <c r="E72" s="25"/>
-      <c r="F72" s="25"/>
-      <c r="G72" s="25"/>
-    </row>
-    <row r="73" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A73" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
-      <c r="E73" s="25"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="25"/>
-    </row>
-    <row r="74" spans="1:7" ht="46.5" customHeight="1">
-      <c r="A74" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
-    </row>
-    <row r="75" spans="1:7" ht="47.25" customHeight="1">
-      <c r="A75" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="25"/>
-      <c r="E75" s="25"/>
-      <c r="F75" s="25"/>
-      <c r="G75" s="25"/>
-    </row>
-    <row r="76" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A76" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
-      <c r="G76" s="25"/>
-    </row>
-    <row r="77" spans="1:7" ht="69.75" customHeight="1">
-      <c r="A77" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="25"/>
-      <c r="F77" s="25"/>
-      <c r="G77" s="25"/>
-    </row>
-    <row r="78" spans="1:7" ht="48" customHeight="1">
-      <c r="A78" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="25"/>
-      <c r="F78" s="25"/>
-      <c r="G78" s="25"/>
-    </row>
-    <row r="79" spans="1:7" ht="15.75">
-      <c r="A79" s="25"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="25"/>
+      <c r="B79" s="31"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="31"/>
+      <c r="E79" s="31"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="31"/>
     </row>
     <row r="80" spans="1:7" ht="15.75">
-      <c r="A80" s="25"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
+      <c r="A80" s="31"/>
+      <c r="B80" s="31"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="31"/>
+      <c r="E80" s="31"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="31"/>
+    </row>
+    <row r="81" spans="1:7" ht="15.75">
+      <c r="A81" s="31"/>
+      <c r="B81" s="31"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="31"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="31"/>
+      <c r="G81" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A77:G77"/>
     <mergeCell ref="A78:G78"/>
     <mergeCell ref="A79:G79"/>
     <mergeCell ref="A80:G80"/>
-    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A81:G81"/>
     <mergeCell ref="A73:G73"/>
     <mergeCell ref="A74:G74"/>
     <mergeCell ref="A75:G75"/>
     <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="A77:G77"/>
     <mergeCell ref="A68:G68"/>
     <mergeCell ref="A69:G69"/>
     <mergeCell ref="A70:G70"/>
     <mergeCell ref="A71:G71"/>
-    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A72:G72"/>
     <mergeCell ref="A61:G61"/>
     <mergeCell ref="A62:G62"/>
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A65:G65"/>
     <mergeCell ref="A56:G56"/>
     <mergeCell ref="A57:G57"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A44:G44"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A54:G54"/>
     <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A55:G55"/>
     <mergeCell ref="A37:G37"/>
     <mergeCell ref="A38:G38"/>
     <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A29:G29"/>
     <mergeCell ref="A30:G30"/>
     <mergeCell ref="A31:G31"/>
     <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A35:G35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2119,21 +2151,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="58.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="13.140625" customWidth="1"/>
   </cols>
@@ -2171,19 +2203,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="31.5">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="36" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="11" t="s">
@@ -2198,16 +2230,16 @@
       <c r="I2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="J2" s="36" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="30"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="11" t="s">
         <v>23</v>
       </c>
@@ -2220,70 +2252,36 @@
       <c r="I3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="30"/>
-    </row>
-    <row r="4" spans="1:10" ht="132" customHeight="1" thickBot="1">
-      <c r="A4" s="14"/>
+      <c r="J3" s="37"/>
+    </row>
+    <row r="4" spans="1:10" ht="378.75" thickBot="1">
+      <c r="A4" s="14">
+        <v>1</v>
+      </c>
       <c r="B4" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>111</v>
+        <v>98</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>135</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>112</v>
+        <v>136</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="H4" s="23"/>
       <c r="I4" s="23" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="17"/>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A6" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2300,12 +2298,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -2346,28 +2342,28 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="36" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="36" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -2375,145 +2371,157 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
       <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" ht="59.25" customHeight="1" thickBot="1">
-      <c r="A5" s="14"/>
+      <c r="A5" s="14">
+        <v>1</v>
+      </c>
       <c r="B5" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>72</v>
+        <v>155</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" ht="103.5" customHeight="1" thickBot="1">
-      <c r="A6" s="14"/>
+      <c r="A6" s="14">
+        <v>2</v>
+      </c>
       <c r="B6" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" ht="149.25" customHeight="1" thickBot="1">
-      <c r="A7" s="14"/>
+      <c r="A7" s="14">
+        <v>3</v>
+      </c>
       <c r="B7" s="19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9" ht="75" customHeight="1" thickBot="1">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14">
+        <v>4</v>
+      </c>
       <c r="B8" s="19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" ht="142.5" thickBot="1">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:9" ht="111" thickBot="1">
+      <c r="A9" s="14">
+        <v>5</v>
+      </c>
       <c r="B9" s="19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A10" s="14"/>
+      <c r="A10" s="14">
+        <v>6</v>
+      </c>
       <c r="B10" s="19" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="19" t="s">
@@ -2521,18 +2529,20 @@
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="95.25" thickBot="1">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14">
+        <v>7</v>
+      </c>
       <c r="B11" s="19" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="19" t="s">
@@ -2540,18 +2550,20 @@
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" ht="95.25" thickBot="1">
-      <c r="A12" s="14"/>
+      <c r="A12" s="14">
+        <v>8</v>
+      </c>
       <c r="B12" s="19" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="19" t="s">
@@ -2559,7 +2571,7 @@
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
@@ -2638,104 +2650,106 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="58.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="40" t="s">
         <v>34</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="40" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
       <c r="I2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="34"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="41"/>
     </row>
     <row r="3" spans="1:12" ht="31.5">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="36" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="36" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="10" t="s">
@@ -2750,22 +2764,22 @@
       <c r="J3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="31" t="s">
+      <c r="K3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="29" t="s">
+      <c r="L3" s="36" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="10" t="s">
         <v>23</v>
       </c>
@@ -2778,198 +2792,212 @@
       <c r="J4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="30"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="37"/>
     </row>
     <row r="5" spans="1:12" ht="80.25" customHeight="1">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+    </row>
+    <row r="6" spans="1:12" ht="80.25" customHeight="1">
+      <c r="A6" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="25"/>
+    </row>
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="L7" s="25"/>
+    </row>
+    <row r="8" spans="1:12" ht="30">
+      <c r="A8" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="L8" s="25"/>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B9" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9" s="25"/>
+    </row>
+    <row r="10" spans="1:12" ht="30">
+      <c r="A10" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38" t="s">
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38" t="s">
+      <c r="L10" s="25"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="L5" s="38"/>
-    </row>
-    <row r="6" spans="1:12" ht="45">
-      <c r="A6" s="38" t="s">
+      <c r="B11" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="38" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" s="25"/>
+    </row>
+    <row r="12" spans="1:12" ht="60">
+      <c r="A12" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38" t="s">
+      <c r="B12" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="L6" s="38"/>
-    </row>
-    <row r="7" spans="1:12" ht="30">
-      <c r="A7" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="L7" s="38"/>
-    </row>
-    <row r="8" spans="1:12" ht="30">
-      <c r="A8" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="38" t="s">
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="L12" s="25"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="25" t="s">
         <v>102</v>
-      </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38" t="s">
-        <v>97</v>
-      </c>
-      <c r="L8" s="38"/>
-    </row>
-    <row r="9" spans="1:12" ht="30">
-      <c r="A9" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="L9" s="38"/>
-    </row>
-    <row r="10" spans="1:12" ht="30">
-      <c r="A10" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="L10" s="38"/>
-    </row>
-    <row r="11" spans="1:12" ht="60">
-      <c r="A11" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>109</v>
-      </c>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="L11" s="38"/>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>116</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>149</v>
+      </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
@@ -2978,18 +3006,20 @@
       <c r="L13" s="14"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>119</v>
+      <c r="A14" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>102</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>149</v>
+      </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -2998,12 +3028,20 @@
       <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>105</v>
+      </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>149</v>
+      </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
@@ -3012,8 +3050,8 @@
       <c r="L15" s="14"/>
     </row>
     <row r="17" spans="1:1" ht="15.75">
-      <c r="A17" s="39" t="s">
-        <v>115</v>
+      <c r="A17" s="26" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75">
@@ -3021,7 +3059,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="D1:D2"/>
@@ -3039,6 +3076,7 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="C1:C2"/>
+    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3046,11 +3084,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3088,25 +3126,25 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="36" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="36" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -3114,29 +3152,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="48" thickBot="1">
@@ -3163,14 +3201,14 @@
         <v>63</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>64</v>
+        <v>150</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3178,17 +3216,17 @@
     <row r="7" spans="1:8" ht="48" thickBot="1">
       <c r="A7" s="14"/>
       <c r="B7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>67</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3196,10 +3234,10 @@
     <row r="8" spans="1:8" ht="48" thickBot="1">
       <c r="A8" s="14"/>
       <c r="B8" s="19" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="19" t="s">

</xml_diff>

<commit_message>
Updated ControlRouteSuitability document, candidate for review.
</commit_message>
<xml_diff>
--- a/System Analysis/WorkingRepository/Group1/ControlRouteSuitability.xlsx
+++ b/System Analysis/WorkingRepository/Group1/ControlRouteSuitability.xlsx
@@ -14,14 +14,14 @@
     <sheet name="Exported Requirements" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="__DdeLink__1724_1104613906" localSheetId="2">Requirements!$B$5</definedName>
+    <definedName name="__DdeLink__1724_1104613906" localSheetId="2">Requirements!#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="174">
   <si>
     <t>Authors:</t>
   </si>
@@ -304,18 +304,12 @@
     <t>SA-1</t>
   </si>
   <si>
-    <t>SRS-3.12.2.3</t>
-  </si>
-  <si>
     <t>Kernel</t>
   </si>
   <si>
     <t>SA-2</t>
   </si>
   <si>
-    <t>SRS-3.12.2.3, SRS-7.4.2.21</t>
-  </si>
-  <si>
     <t>SA-3</t>
   </si>
   <si>
@@ -325,24 +319,6 @@
     <t>SA-5</t>
   </si>
   <si>
-    <t>SRS-3.12.2.4</t>
-  </si>
-  <si>
-    <t>SRS-4.5.2</t>
-  </si>
-  <si>
-    <t>Function RouteSuitability shall be active in FS, LS and OS modes.</t>
-  </si>
-  <si>
-    <t>SRS-3.12.2.10</t>
-  </si>
-  <si>
-    <t>The train is permitted to run without any route suitability data given from the track. No default values shall be used or supervised by the on-board equipment, i.e. the initial state is that no restrictions related to route suitability exists.</t>
-  </si>
-  <si>
-    <t>SRS-4.10.1.3</t>
-  </si>
-  <si>
     <t>RouteSuitabilityData</t>
   </si>
   <si>
@@ -355,9 +331,6 @@
     <t xml:space="preserve">SRS-3.12.2.1, </t>
   </si>
   <si>
-    <t>SA-1, SA-2, SA-3, SA-4</t>
-  </si>
-  <si>
     <t>List of route suitabilities where incompatibilities occur for this train.</t>
   </si>
   <si>
@@ -373,9 +346,6 @@
     <t>Location to which the train is permitted to proceed and where target speed = zero.</t>
   </si>
   <si>
-    <t>SA-5, SA-8</t>
-  </si>
-  <si>
     <t>SupervisedLocation</t>
   </si>
   <si>
@@ -389,17 +359,6 @@
   </si>
   <si>
     <t>ControlRouteSuitability</t>
-  </si>
-  <si>
-    <t>SA-1, 
-SA-2, 
-SA-3, 
-SA-4, 
-SA-5</t>
-  </si>
-  <si>
-    <t>When entering mode FS, LS, OS or PT, stored route suitability data shall remain unchanged.
-When entering any other mode (except non-relevant modes SF and IS), it shall be deleted.</t>
   </si>
   <si>
     <t>The inputs and outputs data types of the « control route suitability » function are summarised in the SysML diagram below :</t>
@@ -458,9 +417,6 @@
     <t>More precisely, regarding the inputs :</t>
   </si>
   <si>
-    <t>The route suitability data refers initially to a balise group reference NID_LRBG for the start location of the route suitability information. This trackside reference is converted into a unique onboard reference REF corresponding to the last valid balise group crossed by ETCS onboard equipment. The function « determine train location » (not represented on the figure) relocates the train on the balise group but also relocates all trackside profile data on the new reference REF taking into account the linking information between the balise groups.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">With this principle, « control route suitability » and « perform train </t>
     </r>
@@ -620,20 +576,6 @@
     </r>
   </si>
   <si>
-    <t>* Initially, there is no route suitability restriction [3.12.2.10]
-* When the function receives new route suitability data [3.12.2.2], the new identified route unsuitability information of any type (loading gauge or traction system or axle load) shall replace all stored route unsuitability information of the same type.
-* The function shall delete the stored route suitability data from a given location, if required by another function (location to shorten track information [A3.4])
-* The function shall delete the stored route suitability data when it detects a change of mode according to the conditions defined in [4.10].
-* The function shall check route suitability data in FS, LS and OS mode [4.5.2]
-* The function shall check if the train is suitable with respect to the received route suitability data as follows [3.12.2.3] :
-    a. there is a route unsuitability if the loading gauge of the train M_LOADINGGAUGE is not in the list of loading gauges supported by the track (M_LINEGAUGE).
-    b. there is a route unsuitability if the axle load category of the train is above the permitted one received from trackside, (M_AXLELOADCAT).
-    c. there is a route unsuitability if the list of traction systems supported by the train does not include the traction system supported by the track (M_VOLTAGE and NID_CTRACTION)
-* In case of unsuitability [3.12.2.4]:
-    a. The driver shall be informed by a text message (one per type of unsuitability) about all new route unsuitabilities (corresponding to the current train data) at their reception. This displayed information shall be re-evaluated at each reception of new route unsuitability information.
-    b. The location where the closest route unsuitability begins shall be identified (closest unsuitability location) as EOA/SVL to allow train supervision functions to avoid the entry of the train in the unsuitable area.</t>
-  </si>
-  <si>
     <t>Mode, TrainSuitabilityData, RouteSuitabilityData, LocationToShortenTrack</t>
   </si>
   <si>
@@ -682,22 +624,116 @@
     <t>Kernel (but other function)</t>
   </si>
   <si>
-    <t>a) The Kernel shall add an unsuitability to the list of unsuitabilities if TrainSuitabilityData.LoadingGauge is not in the list indicated by RouteSuitabilityData.LineGauges.</t>
-  </si>
-  <si>
-    <t>b) The Kernel shall add an unsuitability to the list Unsuitabilities if the RouteSuitabilityData.TractionSystem is not in TrainSuitabilityData.TractionSystems</t>
-  </si>
-  <si>
-    <t>c) The Kernel shall add an unsuitability to the list Unsuitabilities if TrainSuitabilityData.AxleLoadCategory &gt; RouteSuitabilityData.MaxAxleLoadCategory</t>
-  </si>
-  <si>
-    <t>The Kernel shall compare RouteSuitabilityData with TrainSuitabilityData, and build the list of unsuitabilities (if any).</t>
-  </si>
-  <si>
-    <t>If Unsuitabilities contains at least one unsuitability, the Kernel shall set ClosestUnsuitabilityLocation with the closest location corresponding to the unsuitabilities of the list, and take this location into account when computing EndOfAuthority, SupervisedLocation, and ReleaseSpeed.</t>
-  </si>
-  <si>
     <t>20/11/2013 - v7 - Updated functions, requirements and variables regarding the SysML model</t>
+  </si>
+  <si>
+    <t>LocationToShortenTrack</t>
+  </si>
+  <si>
+    <t>Location to shorten track information represents a location where MA, track description and linking information must be deleted (see 026-A3.4 Handling of Accepted and Stored Information in specific Situations)</t>
+  </si>
+  <si>
+    <t>The route suitability data refers initially to a balise group reference NID_LRBG for the start location of the route suitability information. This trackside reference is converted into a unique onboard reference REF corresponding to the last valid balise group crossed by ETCS onboard equipment. The function « determine train location » relocates the train on the balise group but also relocates all trackside profile data on the new reference REF taking into account the linking information between the balise groups.</t>
+  </si>
+  <si>
+    <t>Initially, there is no route suitability restriction.</t>
+  </si>
+  <si>
+    <t>Subset-26</t>
+  </si>
+  <si>
+    <t>When the function receives new route suitability data, the new identified route unsuitability information of any type (loading gauge or traction system or axle load) shall replace all stored route unsuitability information of the same type.</t>
+  </si>
+  <si>
+    <t>The function shall delete the stored route suitability data from a given location, if required by another function (location to shorten track information).</t>
+  </si>
+  <si>
+    <t>A3.4</t>
+  </si>
+  <si>
+    <t>3.12.2.2</t>
+  </si>
+  <si>
+    <t>3.12.2.10</t>
+  </si>
+  <si>
+    <t>The function shall check route suitability data in FS, LS and OS mode.</t>
+  </si>
+  <si>
+    <t>4.5.2</t>
+  </si>
+  <si>
+    <t>3.12.2.3</t>
+  </si>
+  <si>
+    <t>The function shall check if the train is suitable (TrainSuitabilityData) with respect to the received route suitability data (RouteSuitabilityData) as follows :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a. there is a route unsuitability if the loading gauge of the train M_LOADINGGAUGE (TrainSuitabilityData.LoadingGauge) is not in the list of loading gauges supported by the track (M_LINEGAUGE) (RouteSuitabilityData.LineGauges).</t>
+  </si>
+  <si>
+    <t>3.12.2.3, 7.4.2.21</t>
+  </si>
+  <si>
+    <t>SA-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   b. there is a route unsuitability if the list of traction systems supported by the train (TrainSuitabilityData.TractionSystems) does not include the traction system supported by the track (M_VOLTAGE and NID_CTRACTION) (RouteSuitabilityData.TractionSystem)</t>
+  </si>
+  <si>
+    <t>SA-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    c. there is a route unsuitability if the axle load category of the train is above the permitted one received from trackside, (M_AXLELOADCAT) (TrainSuitabilityData.AxleLoadCategory &gt; RouteSuitabilityData.MaxAxleLoadCategory)</t>
+  </si>
+  <si>
+    <t>SA-10</t>
+  </si>
+  <si>
+    <t>In case of unsuitability :</t>
+  </si>
+  <si>
+    <t>3.12.2.4</t>
+  </si>
+  <si>
+    <t>SA-11</t>
+  </si>
+  <si>
+    <t>SA-12</t>
+  </si>
+  <si>
+    <t>SA-13</t>
+  </si>
+  <si>
+    <t>4.10.1.3</t>
+  </si>
+  <si>
+    <t>The function shall delete the stored route suitability data when it detects a change of mode : when entering any other mode than (except non-relevant modes SF and IS), it shall remove the data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    b. The location where the closest route unsuitability begins shall be identified (ClosestUnsuitabilityLocation) as EOA/SVL to allow train supervision functions to avoid the entry of the train in the unsuitable area.</t>
+  </si>
+  <si>
+    <t>SA-1, SA-2, SA-3, SA-4, SA-5, SA-6, SA-7, SA-8, SA-9, SA-10, SA-11, SA-12, SA-13</t>
+  </si>
+  <si>
+    <t>The implementation of the « control route suitability » function in an interoperable kernel permits to deal with route suitability data when required by a given infrastructure.
+This function manages 3 cases of route unsuitabilities:
+* loading gauge profile of the train not compatible with the line gauge authorised by infrastructure,
+* traction system of the train not compatible with the country traction system
+*  the train axle load category is higher than the maximum authorised by infrastructure</t>
+  </si>
+  <si>
+    <t>SA-5, SA-6</t>
+  </si>
+  <si>
+    <t>SA-7, SA-8, SA-9, SA-10</t>
+  </si>
+  <si>
+    <t>SA-7, SA-8, SA-9, SA-10, SA-11, SA-12, SA-13</t>
+  </si>
+  <si>
+    <t>21/11/2013 - v8 - Uniformized functions, requirements and variables with the description sheet.</t>
   </si>
 </sst>
 </file>
@@ -993,10 +1029,10 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FF000001"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1004,7 +1040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1058,15 +1094,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1089,11 +1116,32 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1103,9 +1151,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1151,13 +1196,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>142873</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>625429</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>3328587</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1184,7 +1229,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1204,13 +1249,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>500380</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>143510</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1222,7 +1267,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1530,24 +1575,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="1"/>
@@ -1566,7 +1611,7 @@
     <row r="6" spans="1:7" ht="15.75">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:7" s="29" customFormat="1" ht="15.75">
+    <row r="7" spans="1:7" s="26" customFormat="1" ht="15.75">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1625,60 +1670,54 @@
     </row>
     <row r="20" spans="1:7" ht="15.75">
       <c r="A20" s="17" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75">
       <c r="A21" s="17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="16.5">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="18.75">
-      <c r="A23" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75">
+      <c r="A22" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16.5">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="18.75">
+      <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75">
-      <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75">
-      <c r="A25" s="17" t="s">
-        <v>47</v>
-      </c>
+    <row r="25" spans="1:7" ht="18.75">
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="15.75">
       <c r="A26" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75">
+      <c r="A27" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75">
-      <c r="A27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" ht="18.75">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:7" ht="15.75">
+      <c r="A28" s="17"/>
     </row>
     <row r="29" spans="1:7" ht="18.75">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="18.75">
+      <c r="A30" s="18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A30" s="30" t="s">
+    <row r="31" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A31" s="34" t="s">
         <v>50</v>
-      </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-    </row>
-    <row r="31" spans="1:7" ht="21.75" customHeight="1">
-      <c r="A31" s="33" t="s">
-        <v>58</v>
       </c>
       <c r="B31" s="34"/>
       <c r="C31" s="34"/>
@@ -1687,462 +1726,473 @@
       <c r="F31" s="34"/>
       <c r="G31" s="34"/>
     </row>
-    <row r="32" spans="1:7" ht="40.5" customHeight="1">
-      <c r="A32" s="33" t="s">
+    <row r="32" spans="1:7" ht="21.75" customHeight="1">
+      <c r="A32" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+    </row>
+    <row r="33" spans="1:7" ht="40.5" customHeight="1">
+      <c r="A33" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-    </row>
-    <row r="33" spans="1:7" ht="53.25" customHeight="1">
-      <c r="A33" s="34" t="s">
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+    </row>
+    <row r="34" spans="1:7" ht="53.25" customHeight="1">
+      <c r="A34" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75">
-      <c r="A34" s="17"/>
-    </row>
-    <row r="35" spans="1:7" ht="60.75" customHeight="1">
-      <c r="A35" s="30" t="s">
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75">
+      <c r="A35" s="17"/>
+    </row>
+    <row r="36" spans="1:7" ht="60.75" customHeight="1">
+      <c r="A36" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75">
-      <c r="A36" s="17"/>
-    </row>
-    <row r="37" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A37" s="30" t="s">
+      <c r="B36" s="34"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="34"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75">
+      <c r="A37" s="17"/>
+    </row>
+    <row r="38" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A38" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-    </row>
-    <row r="38" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A38" s="31" t="s">
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
+      <c r="G38" s="34"/>
+    </row>
+    <row r="39" spans="1:7" ht="35.25" customHeight="1">
+      <c r="A39" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-    </row>
-    <row r="39" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A39" s="30" t="s">
+      <c r="B39" s="34"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="34"/>
+    </row>
+    <row r="40" spans="1:7" ht="28.5" customHeight="1">
+      <c r="A40" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-    </row>
-    <row r="40" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A40" s="30" t="s">
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+    </row>
+    <row r="41" spans="1:7" ht="26.25" customHeight="1">
+      <c r="A41" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75">
-      <c r="A41" s="17"/>
-    </row>
-    <row r="42" spans="1:7" ht="18.75">
-      <c r="A42" s="18" t="s">
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75">
+      <c r="A42" s="17"/>
+    </row>
+    <row r="43" spans="1:7" ht="18.75">
+      <c r="A43" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75">
+      <c r="A44" s="24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="48" customHeight="1">
+      <c r="A45" s="34" t="s">
+        <v>98</v>
+      </c>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.75">
+      <c r="A46" s="17"/>
+    </row>
+    <row r="47" spans="1:7" ht="279.75" customHeight="1">
+      <c r="A47" s="35"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.75">
+      <c r="A53" s="17"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75">
+      <c r="A54" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+    </row>
+    <row r="55" spans="1:7" ht="66" customHeight="1">
+      <c r="A55" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B55" s="33"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="33"/>
+    </row>
+    <row r="56" spans="1:7" ht="46.5" customHeight="1">
+      <c r="A56" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="33"/>
+    </row>
+    <row r="57" spans="1:7" ht="52.5" customHeight="1">
+      <c r="A57" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B57" s="33"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="33"/>
+    </row>
+    <row r="58" spans="1:7" ht="51" customHeight="1">
+      <c r="A58" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B58" s="33"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.75">
+      <c r="A59" s="33"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="33"/>
+      <c r="D59" s="33"/>
+      <c r="E59" s="33"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="33"/>
+    </row>
+    <row r="60" spans="1:7" ht="123.75" customHeight="1">
+      <c r="A60" s="33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" s="33"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="33"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.75">
+      <c r="A61" s="33"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="33"/>
+      <c r="E61" s="33"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="33"/>
+    </row>
+    <row r="62" spans="1:7" ht="42" customHeight="1">
+      <c r="A62" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" s="33"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="33"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.75">
+      <c r="A63" s="33"/>
+      <c r="B63" s="33"/>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="33"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="33"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.75">
+      <c r="A64" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
+      <c r="D64" s="33"/>
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="33"/>
+    </row>
+    <row r="65" spans="1:7" ht="15.75">
+      <c r="A65" s="33" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75">
-      <c r="A43" s="27" t="s">
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
+    </row>
+    <row r="66" spans="1:7" ht="33.75" customHeight="1">
+      <c r="A66" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="33"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="33"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.75">
+      <c r="A67" s="25"/>
+    </row>
+    <row r="68" spans="1:7" ht="15.75">
+      <c r="A68" s="24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A69" s="33" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="48" customHeight="1">
-      <c r="A44" s="30" t="s">
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="33"/>
+    </row>
+    <row r="70" spans="1:7" ht="51.75" customHeight="1">
+      <c r="A70" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
-      <c r="E44" s="30"/>
-      <c r="F44" s="30"/>
-      <c r="G44" s="30"/>
-    </row>
-    <row r="45" spans="1:7" ht="15.75">
-      <c r="A45" s="17"/>
-    </row>
-    <row r="46" spans="1:7" ht="279.75" customHeight="1">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-    </row>
-    <row r="52" spans="1:7" ht="15.75">
-      <c r="A52" s="17"/>
-    </row>
-    <row r="53" spans="1:7" ht="15.75">
-      <c r="A53" s="31" t="s">
+      <c r="B70" s="33"/>
+      <c r="C70" s="33"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="33"/>
+    </row>
+    <row r="71" spans="1:7" ht="40.5" customHeight="1">
+      <c r="A71" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="31"/>
-    </row>
-    <row r="54" spans="1:7" ht="66" customHeight="1">
-      <c r="A54" s="31" t="s">
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="33"/>
+    </row>
+    <row r="72" spans="1:7" ht="36" customHeight="1">
+      <c r="A72" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B72" s="33"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="33"/>
+    </row>
+    <row r="73" spans="1:7" ht="20.25" customHeight="1">
+      <c r="A73" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="33"/>
+    </row>
+    <row r="74" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A74" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="B74" s="33"/>
+      <c r="C74" s="33"/>
+      <c r="D74" s="33"/>
+      <c r="E74" s="33"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="33"/>
+    </row>
+    <row r="75" spans="1:7" ht="37.5" customHeight="1">
+      <c r="A75" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B75" s="33"/>
+      <c r="C75" s="33"/>
+      <c r="D75" s="33"/>
+      <c r="E75" s="33"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="33"/>
+    </row>
+    <row r="76" spans="1:7" ht="46.5" customHeight="1">
+      <c r="A76" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="31"/>
-    </row>
-    <row r="55" spans="1:7" ht="46.5" customHeight="1">
-      <c r="A55" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="31"/>
-    </row>
-    <row r="56" spans="1:7" ht="52.5" customHeight="1">
-      <c r="A56" s="31" t="s">
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="33"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="33"/>
+    </row>
+    <row r="77" spans="1:7" ht="47.25" customHeight="1">
+      <c r="A77" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="B77" s="33"/>
+      <c r="C77" s="33"/>
+      <c r="D77" s="33"/>
+      <c r="E77" s="33"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="33"/>
+    </row>
+    <row r="78" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A78" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
+      <c r="D78" s="33"/>
+      <c r="E78" s="33"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="33"/>
+    </row>
+    <row r="79" spans="1:7" ht="69.75" customHeight="1">
+      <c r="A79" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-    </row>
-    <row r="57" spans="1:7" ht="51" customHeight="1">
-      <c r="A57" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-    </row>
-    <row r="58" spans="1:7" ht="15.75">
-      <c r="A58" s="31"/>
-      <c r="B58" s="31"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="31"/>
-    </row>
-    <row r="59" spans="1:7" ht="123.75" customHeight="1">
-      <c r="A59" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-    </row>
-    <row r="60" spans="1:7" ht="15.75">
-      <c r="A60" s="31"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-    </row>
-    <row r="61" spans="1:7" ht="42" customHeight="1">
-      <c r="A61" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="31"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31"/>
-    </row>
-    <row r="62" spans="1:7" ht="15.75">
-      <c r="A62" s="31"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="31"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31"/>
-    </row>
-    <row r="63" spans="1:7" ht="15.75">
-      <c r="A63" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-    </row>
-    <row r="64" spans="1:7" ht="15.75">
-      <c r="A64" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="31"/>
-    </row>
-    <row r="65" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A65" s="31" t="s">
+      <c r="B79" s="33"/>
+      <c r="C79" s="33"/>
+      <c r="D79" s="33"/>
+      <c r="E79" s="33"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="33"/>
+    </row>
+    <row r="80" spans="1:7" ht="48" customHeight="1">
+      <c r="A80" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="B65" s="31"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="31"/>
-      <c r="E65" s="31"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="31"/>
-    </row>
-    <row r="66" spans="1:7" ht="15.75">
-      <c r="A66" s="28"/>
-    </row>
-    <row r="67" spans="1:7" ht="15.75">
-      <c r="A67" s="27" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A68" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-    </row>
-    <row r="69" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A69" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="31"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="31"/>
-    </row>
-    <row r="70" spans="1:7" ht="40.5" customHeight="1">
-      <c r="A70" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="31"/>
-    </row>
-    <row r="71" spans="1:7" ht="36" customHeight="1">
-      <c r="A71" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-    </row>
-    <row r="72" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A72" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="B72" s="31"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="31"/>
-      <c r="E72" s="31"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31"/>
-    </row>
-    <row r="73" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A73" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="B73" s="31"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="31"/>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-    </row>
-    <row r="74" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A74" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="B74" s="31"/>
-      <c r="C74" s="31"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31"/>
-    </row>
-    <row r="75" spans="1:7" ht="46.5" customHeight="1">
-      <c r="A75" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B75" s="31"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="31"/>
-    </row>
-    <row r="76" spans="1:7" ht="47.25" customHeight="1">
-      <c r="A76" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="B76" s="31"/>
-      <c r="C76" s="31"/>
-      <c r="D76" s="31"/>
-      <c r="E76" s="31"/>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31"/>
-    </row>
-    <row r="77" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A77" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B77" s="31"/>
-      <c r="C77" s="31"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="31"/>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31"/>
-    </row>
-    <row r="78" spans="1:7" ht="69.75" customHeight="1">
-      <c r="A78" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="B78" s="31"/>
-      <c r="C78" s="31"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31"/>
-    </row>
-    <row r="79" spans="1:7" ht="48" customHeight="1">
-      <c r="A79" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="B79" s="31"/>
-      <c r="C79" s="31"/>
-      <c r="D79" s="31"/>
-      <c r="E79" s="31"/>
-      <c r="F79" s="31"/>
-      <c r="G79" s="31"/>
-    </row>
-    <row r="80" spans="1:7" ht="15.75">
-      <c r="A80" s="31"/>
-      <c r="B80" s="31"/>
-      <c r="C80" s="31"/>
-      <c r="D80" s="31"/>
-      <c r="E80" s="31"/>
-      <c r="F80" s="31"/>
-      <c r="G80" s="31"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
+      <c r="D80" s="33"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
     </row>
     <row r="81" spans="1:7" ht="15.75">
-      <c r="A81" s="31"/>
-      <c r="B81" s="31"/>
-      <c r="C81" s="31"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="31"/>
-      <c r="F81" s="31"/>
-      <c r="G81" s="31"/>
+      <c r="A81" s="33"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="33"/>
+      <c r="E81" s="33"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="33"/>
+    </row>
+    <row r="82" spans="1:7" ht="15.75">
+      <c r="A82" s="33"/>
+      <c r="B82" s="33"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="33"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="A79:G79"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A75:G75"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A68:G68"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="A60:G60"/>
     <mergeCell ref="A61:G61"/>
     <mergeCell ref="A62:G62"/>
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="A64:G64"/>
     <mergeCell ref="A65:G65"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A57:G57"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="A79:G79"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A78:G78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2154,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2203,19 +2253,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="31.5">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="39" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="11" t="s">
@@ -2230,16 +2280,16 @@
       <c r="I2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="36" t="s">
+      <c r="J2" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="37"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="40"/>
       <c r="F3" s="11" t="s">
         <v>23</v>
       </c>
@@ -2252,33 +2302,33 @@
       <c r="I3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="37"/>
-    </row>
-    <row r="4" spans="1:10" ht="378.75" thickBot="1">
+      <c r="J3" s="40"/>
+    </row>
+    <row r="4" spans="1:10" ht="174" thickBot="1">
       <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>137</v>
-      </c>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" s="22"/>
+      <c r="B4" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="17"/>
@@ -2299,9 +2349,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -2342,28 +2394,28 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="36" t="s">
+      <c r="H2" s="39" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="12" t="s">
@@ -2371,282 +2423,380 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
       <c r="I3" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="59.25" customHeight="1" thickBot="1">
-      <c r="A5" s="14">
+    <row r="5" spans="1:9" ht="15.75">
+      <c r="A5" s="29">
         <v>1</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="G5" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
+    </row>
+    <row r="6" spans="1:9" ht="94.5">
+      <c r="A6" s="29">
+        <v>2</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:9" ht="94.5">
+      <c r="A7" s="29">
+        <v>3</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" ht="63">
+      <c r="A8" s="29">
+        <v>4</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" ht="78.75">
+      <c r="A9" s="29">
+        <v>5</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="1:9" ht="31.5">
+      <c r="A10" s="29">
+        <v>6</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="30"/>
+    </row>
+    <row r="11" spans="1:9" ht="63">
+      <c r="A11" s="29">
+        <v>7</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
+    </row>
+    <row r="12" spans="1:9" ht="94.5">
+      <c r="A12" s="29">
+        <v>8</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="19" t="s">
+      <c r="C12" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="G12" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-    </row>
-    <row r="6" spans="1:9" ht="103.5" customHeight="1" thickBot="1">
-      <c r="A6" s="14">
-        <v>2</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="1:9" ht="149.25" customHeight="1" thickBot="1">
-      <c r="A7" s="14">
-        <v>3</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-    </row>
-    <row r="8" spans="1:9" ht="75" customHeight="1" thickBot="1">
-      <c r="A8" s="14">
-        <v>4</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="19" t="s">
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
+    </row>
+    <row r="13" spans="1:9" ht="110.25">
+      <c r="A13" s="29">
+        <v>9</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:9" ht="111" thickBot="1">
-      <c r="A9" s="14">
-        <v>5</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="1:9" ht="32.25" thickBot="1">
-      <c r="A10" s="14">
-        <v>6</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="1:9" ht="95.25" thickBot="1">
-      <c r="A11" s="14">
-        <v>7</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="1:9" ht="95.25" thickBot="1">
-      <c r="A12" s="14">
-        <v>8</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="G13" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14" spans="1:9" ht="110.25">
+      <c r="A14" s="29">
+        <v>10</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>158</v>
+      </c>
       <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
+      <c r="E14" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>70</v>
+      </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="1:9">
+    <row r="15" spans="1:9" ht="15.75">
+      <c r="A15" s="29">
+        <v>11</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+    </row>
+    <row r="16" spans="1:9" ht="110.25">
+      <c r="A16" s="29">
+        <v>12</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+    </row>
+    <row r="17" spans="1:9" ht="78.75">
+      <c r="A17" s="29">
+        <v>13</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75">
       <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="E18" s="27"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
     </row>
+    <row r="19" spans="1:9" ht="15.75">
+      <c r="A19" s="17"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+    </row>
     <row r="20" spans="1:9" ht="15.75">
-      <c r="A20" s="17"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
     </row>
     <row r="21" spans="1:9" ht="15.75">
-      <c r="A21" s="17"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75">
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75">
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2659,15 +2809,16 @@
     <mergeCell ref="F2:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2680,76 +2831,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="43" t="s">
         <v>34</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="L1" s="43" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16.5" thickBot="1">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
       <c r="I2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="41"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="41"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="44"/>
     </row>
     <row r="3" spans="1:12" ht="31.5">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="39" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="10" t="s">
@@ -2764,22 +2915,22 @@
       <c r="J3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="L3" s="39" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
       <c r="G4" s="10" t="s">
         <v>23</v>
       </c>
@@ -2792,233 +2943,237 @@
       <c r="J4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="39"/>
-      <c r="L4" s="37"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="40"/>
     </row>
     <row r="5" spans="1:12" ht="80.25" customHeight="1">
-      <c r="A5" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25" t="s">
+      <c r="A5" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="L5" s="22"/>
+    </row>
+    <row r="6" spans="1:12" ht="80.25" customHeight="1">
+      <c r="A6" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="22"/>
+    </row>
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="L7" s="22"/>
+    </row>
+    <row r="8" spans="1:12" ht="60">
+      <c r="A8" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="L9" s="22"/>
+    </row>
+    <row r="10" spans="1:12" ht="60">
+      <c r="A10" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-    </row>
-    <row r="6" spans="1:12" ht="80.25" customHeight="1">
-      <c r="A6" s="25" t="s">
+      <c r="B10" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="L11" s="22"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25" t="s">
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="L12" s="22"/>
+    </row>
+    <row r="13" spans="1:12" ht="60">
+      <c r="A13" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="L6" s="25"/>
-    </row>
-    <row r="7" spans="1:12" ht="30">
-      <c r="A7" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25" t="s">
+      <c r="B13" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="25"/>
-    </row>
-    <row r="8" spans="1:12" ht="30">
-      <c r="A8" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="L8" s="25"/>
-    </row>
-    <row r="9" spans="1:12" ht="30">
-      <c r="A9" s="25" t="s">
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="L13" s="22"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>90</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="L9" s="25"/>
-    </row>
-    <row r="10" spans="1:12" ht="30">
-      <c r="A10" s="25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="L10" s="25"/>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="A11" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25" t="s">
-        <v>93</v>
-      </c>
-      <c r="L11" s="25"/>
-    </row>
-    <row r="12" spans="1:12" ht="60">
-      <c r="A12" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25" t="s">
-        <v>148</v>
-      </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="L12" s="25"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C13" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>102</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -3028,19 +3183,19 @@
       <c r="L14" s="14"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>105</v>
+      <c r="A15" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>90</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="14" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -3049,26 +3204,38 @@
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="17" spans="1:1" ht="15.75">
-      <c r="A17" s="26" t="s">
-        <v>101</v>
-      </c>
+    <row r="16" spans="1:12">
+      <c r="A16" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
     </row>
     <row r="18" spans="1:1" ht="15.75">
-      <c r="A18" s="17"/>
+      <c r="A18" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75">
+      <c r="A19" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="H1:H2"/>
@@ -3077,6 +3244,16 @@
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3085,10 +3262,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3126,25 +3303,25 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="39" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="39" t="s">
         <v>21</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -3152,122 +3329,106 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="13"/>
     </row>
-    <row r="5" spans="1:8" ht="48" thickBot="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="19" t="s">
+    <row r="5" spans="1:8" ht="47.25">
+      <c r="A5" s="14">
+        <v>1</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="28" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="27" t="s">
         <v>62</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" ht="32.25" thickBot="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>150</v>
+    <row r="6" spans="1:8" ht="31.5">
+      <c r="A6" s="14">
+        <v>2</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28" t="s">
+        <v>136</v>
       </c>
       <c r="D6" s="14"/>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="19" t="s">
+      <c r="F6" s="27" t="s">
         <v>64</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
     </row>
-    <row r="7" spans="1:8" ht="48" thickBot="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="20" t="s">
+    <row r="7" spans="1:8" ht="47.25">
+      <c r="A7" s="14">
+        <v>3</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28" t="s">
         <v>66</v>
       </c>
       <c r="D7" s="14"/>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="19" t="s">
-        <v>151</v>
+      <c r="F7" s="27" t="s">
+        <v>137</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
     </row>
-    <row r="8" spans="1:8" ht="48" thickBot="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="19" t="s">
+    <row r="8" spans="1:8" ht="47.25">
+      <c r="A8" s="14">
+        <v>4</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="28" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="27" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Fixed tiny errors in ControlRouteSuitability.
</commit_message>
<xml_diff>
--- a/System Analysis/WorkingRepository/Group1/ControlRouteSuitability.xlsx
+++ b/System Analysis/WorkingRepository/Group1/ControlRouteSuitability.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720"/>
+    <workbookView xWindow="360" yWindow="135" windowWidth="14115" windowHeight="6720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="173">
   <si>
     <t>Authors:</t>
   </si>
@@ -702,19 +702,10 @@
     <t>SA-12</t>
   </si>
   <si>
-    <t>SA-13</t>
-  </si>
-  <si>
     <t>4.10.1.3</t>
   </si>
   <si>
-    <t>The function shall delete the stored route suitability data when it detects a change of mode : when entering any other mode than (except non-relevant modes SF and IS), it shall remove the data.</t>
-  </si>
-  <si>
     <t xml:space="preserve">    b. The location where the closest route unsuitability begins shall be identified (ClosestUnsuitabilityLocation) as EOA/SVL to allow train supervision functions to avoid the entry of the train in the unsuitable area.</t>
-  </si>
-  <si>
-    <t>SA-1, SA-2, SA-3, SA-4, SA-5, SA-6, SA-7, SA-8, SA-9, SA-10, SA-11, SA-12, SA-13</t>
   </si>
   <si>
     <t>The implementation of the « control route suitability » function in an interoperable kernel permits to deal with route suitability data when required by a given infrastructure.
@@ -724,16 +715,22 @@
 *  the train axle load category is higher than the maximum authorised by infrastructure</t>
   </si>
   <si>
-    <t>SA-5, SA-6</t>
-  </si>
-  <si>
-    <t>SA-7, SA-8, SA-9, SA-10</t>
-  </si>
-  <si>
-    <t>SA-7, SA-8, SA-9, SA-10, SA-11, SA-12, SA-13</t>
-  </si>
-  <si>
     <t>21/11/2013 - v8 - Uniformized functions, requirements and variables with the description sheet.</t>
+  </si>
+  <si>
+    <t>The function shall delete the stored route suitability data when it detects a change of mode : when entering any other mode than FS, LS, OS or PT (except non-relevant modes SF and IS), it shall remove the data.</t>
+  </si>
+  <si>
+    <t>SA-4, SA-5</t>
+  </si>
+  <si>
+    <t>SA-6, SA-7, SA-8, SA-9</t>
+  </si>
+  <si>
+    <t>SA-6, SA-7, SA-8, SA-9, SA-10, SA-11, SA-12</t>
+  </si>
+  <si>
+    <t>SA-1, SA-2, SA-3, SA-4, SA-5, SA-6, SA-7, SA-8, SA-9, SA-10, SA-11, SA-12</t>
   </si>
 </sst>
 </file>
@@ -1134,23 +1131,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1229,7 +1226,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1267,7 +1264,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1577,22 +1574,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7" ht="22.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" ht="15.75">
       <c r="A2" s="1"/>
@@ -1680,7 +1677,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75">
       <c r="A22" s="17" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="16.5">
@@ -1716,109 +1713,109 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
     </row>
     <row r="32" spans="1:7" ht="21.75" customHeight="1">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="38"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
     </row>
     <row r="33" spans="1:7" ht="40.5" customHeight="1">
-      <c r="A33" s="37" t="s">
+      <c r="A33" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
     </row>
     <row r="34" spans="1:7" ht="53.25" customHeight="1">
-      <c r="A34" s="38" t="s">
+      <c r="A34" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="37"/>
+      <c r="D34" s="37"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
     </row>
     <row r="35" spans="1:7" ht="15.75">
       <c r="A35" s="17"/>
     </row>
     <row r="36" spans="1:7" ht="60.75" customHeight="1">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
     </row>
     <row r="37" spans="1:7" ht="15.75">
       <c r="A37" s="17"/>
     </row>
     <row r="38" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
     </row>
     <row r="39" spans="1:7" ht="35.25" customHeight="1">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="34"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
     </row>
     <row r="40" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:7" ht="15.75">
       <c r="A42" s="17"/>
@@ -1834,165 +1831,165 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="48" customHeight="1">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
+      <c r="D45" s="33"/>
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="33"/>
     </row>
     <row r="46" spans="1:7" ht="15.75">
       <c r="A46" s="17"/>
     </row>
     <row r="47" spans="1:7" ht="279.75" customHeight="1">
-      <c r="A47" s="35"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
+      <c r="A47" s="38"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
     </row>
     <row r="53" spans="1:7" ht="15.75">
       <c r="A53" s="17"/>
     </row>
     <row r="54" spans="1:7" ht="15.75">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
     </row>
     <row r="55" spans="1:7" ht="66" customHeight="1">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="34"/>
     </row>
     <row r="56" spans="1:7" ht="46.5" customHeight="1">
-      <c r="A56" s="33" t="s">
+      <c r="A56" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="34"/>
+      <c r="G56" s="34"/>
     </row>
     <row r="57" spans="1:7" ht="52.5" customHeight="1">
-      <c r="A57" s="33" t="s">
+      <c r="A57" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
+      <c r="B57" s="34"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="34"/>
+      <c r="G57" s="34"/>
     </row>
     <row r="58" spans="1:7" ht="51" customHeight="1">
-      <c r="A58" s="33" t="s">
+      <c r="A58" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
     </row>
     <row r="59" spans="1:7" ht="15.75">
-      <c r="A59" s="33"/>
-      <c r="B59" s="33"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
+      <c r="A59" s="34"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="34"/>
+      <c r="G59" s="34"/>
     </row>
     <row r="60" spans="1:7" ht="123.75" customHeight="1">
-      <c r="A60" s="33" t="s">
+      <c r="A60" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="B60" s="33"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
+      <c r="B60" s="34"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="34"/>
+      <c r="G60" s="34"/>
     </row>
     <row r="61" spans="1:7" ht="15.75">
-      <c r="A61" s="33"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
+      <c r="A61" s="34"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="34"/>
+      <c r="G61" s="34"/>
     </row>
     <row r="62" spans="1:7" ht="42" customHeight="1">
-      <c r="A62" s="33" t="s">
+      <c r="A62" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="B62" s="33"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
+      <c r="B62" s="34"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="34"/>
+      <c r="G62" s="34"/>
     </row>
     <row r="63" spans="1:7" ht="15.75">
-      <c r="A63" s="33"/>
-      <c r="B63" s="33"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
+      <c r="A63" s="34"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="34"/>
+      <c r="G63" s="34"/>
     </row>
     <row r="64" spans="1:7" ht="15.75">
-      <c r="A64" s="33" t="s">
+      <c r="A64" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="B64" s="33"/>
-      <c r="C64" s="33"/>
-      <c r="D64" s="33"/>
-      <c r="E64" s="33"/>
-      <c r="F64" s="33"/>
-      <c r="G64" s="33"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
     </row>
     <row r="65" spans="1:7" ht="15.75">
-      <c r="A65" s="33" t="s">
+      <c r="A65" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="B65" s="33"/>
-      <c r="C65" s="33"/>
-      <c r="D65" s="33"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="34"/>
+      <c r="G65" s="34"/>
     </row>
     <row r="66" spans="1:7" ht="33.75" customHeight="1">
-      <c r="A66" s="33" t="s">
+      <c r="A66" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B66" s="33"/>
-      <c r="C66" s="33"/>
-      <c r="D66" s="33"/>
-      <c r="E66" s="33"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="33"/>
+      <c r="B66" s="34"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="34"/>
+      <c r="G66" s="34"/>
     </row>
     <row r="67" spans="1:7" ht="15.75">
       <c r="A67" s="25"/>
@@ -2003,157 +2000,186 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A69" s="33" t="s">
+      <c r="A69" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B69" s="33"/>
-      <c r="C69" s="33"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="33"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="33"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="34"/>
+      <c r="G69" s="34"/>
     </row>
     <row r="70" spans="1:7" ht="51.75" customHeight="1">
-      <c r="A70" s="33" t="s">
+      <c r="A70" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="C70" s="33"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="33"/>
+      <c r="B70" s="34"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="34"/>
     </row>
     <row r="71" spans="1:7" ht="40.5" customHeight="1">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
-      <c r="E71" s="33"/>
-      <c r="F71" s="33"/>
-      <c r="G71" s="33"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="34"/>
+      <c r="G71" s="34"/>
     </row>
     <row r="72" spans="1:7" ht="36" customHeight="1">
-      <c r="A72" s="33" t="s">
+      <c r="A72" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="B72" s="33"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="33"/>
-      <c r="F72" s="33"/>
-      <c r="G72" s="33"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
+      <c r="G72" s="34"/>
     </row>
     <row r="73" spans="1:7" ht="20.25" customHeight="1">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="C73" s="33"/>
-      <c r="D73" s="33"/>
-      <c r="E73" s="33"/>
-      <c r="F73" s="33"/>
-      <c r="G73" s="33"/>
+      <c r="B73" s="34"/>
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="34"/>
+      <c r="G73" s="34"/>
     </row>
     <row r="74" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A74" s="33" t="s">
+      <c r="A74" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="B74" s="33"/>
-      <c r="C74" s="33"/>
-      <c r="D74" s="33"/>
-      <c r="E74" s="33"/>
-      <c r="F74" s="33"/>
-      <c r="G74" s="33"/>
+      <c r="B74" s="34"/>
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="34"/>
     </row>
     <row r="75" spans="1:7" ht="37.5" customHeight="1">
-      <c r="A75" s="33" t="s">
+      <c r="A75" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="C75" s="33"/>
-      <c r="D75" s="33"/>
-      <c r="E75" s="33"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="33"/>
+      <c r="B75" s="34"/>
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="34"/>
+      <c r="G75" s="34"/>
     </row>
     <row r="76" spans="1:7" ht="46.5" customHeight="1">
-      <c r="A76" s="33" t="s">
+      <c r="A76" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="C76" s="33"/>
-      <c r="D76" s="33"/>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
+      <c r="B76" s="34"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="34"/>
     </row>
     <row r="77" spans="1:7" ht="47.25" customHeight="1">
-      <c r="A77" s="33" t="s">
+      <c r="A77" s="34" t="s">
         <v>116</v>
       </c>
-      <c r="B77" s="33"/>
-      <c r="C77" s="33"/>
-      <c r="D77" s="33"/>
-      <c r="E77" s="33"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="33"/>
+      <c r="B77" s="34"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="34"/>
+      <c r="G77" s="34"/>
     </row>
     <row r="78" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A78" s="33" t="s">
+      <c r="A78" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="B78" s="33"/>
-      <c r="C78" s="33"/>
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="33"/>
+      <c r="B78" s="34"/>
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="34"/>
+      <c r="G78" s="34"/>
     </row>
     <row r="79" spans="1:7" ht="69.75" customHeight="1">
-      <c r="A79" s="33" t="s">
+      <c r="A79" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="B79" s="33"/>
-      <c r="C79" s="33"/>
-      <c r="D79" s="33"/>
-      <c r="E79" s="33"/>
-      <c r="F79" s="33"/>
-      <c r="G79" s="33"/>
+      <c r="B79" s="34"/>
+      <c r="C79" s="34"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="34"/>
+      <c r="F79" s="34"/>
+      <c r="G79" s="34"/>
     </row>
     <row r="80" spans="1:7" ht="48" customHeight="1">
-      <c r="A80" s="33" t="s">
+      <c r="A80" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="B80" s="33"/>
-      <c r="C80" s="33"/>
-      <c r="D80" s="33"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="33"/>
-      <c r="G80" s="33"/>
+      <c r="B80" s="34"/>
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
     </row>
     <row r="81" spans="1:7" ht="15.75">
-      <c r="A81" s="33"/>
-      <c r="B81" s="33"/>
-      <c r="C81" s="33"/>
-      <c r="D81" s="33"/>
-      <c r="E81" s="33"/>
-      <c r="F81" s="33"/>
-      <c r="G81" s="33"/>
+      <c r="A81" s="34"/>
+      <c r="B81" s="34"/>
+      <c r="C81" s="34"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="34"/>
+      <c r="F81" s="34"/>
+      <c r="G81" s="34"/>
     </row>
     <row r="82" spans="1:7" ht="15.75">
-      <c r="A82" s="33"/>
-      <c r="B82" s="33"/>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="33"/>
-      <c r="F82" s="33"/>
-      <c r="G82" s="33"/>
+      <c r="A82" s="34"/>
+      <c r="B82" s="34"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="34"/>
+      <c r="F82" s="34"/>
+      <c r="G82" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A79:G79"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A56:G56"/>
     <mergeCell ref="A38:G38"/>
     <mergeCell ref="A39:G39"/>
     <mergeCell ref="A40:G40"/>
@@ -2164,35 +2190,6 @@
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A36:G36"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A57:G57"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="A63:G63"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="A72:G72"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="A79:G79"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="A82:G82"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="A75:G75"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="A78:G78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2204,8 +2201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2312,7 +2309,7 @@
         <v>88</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="20" t="s">
@@ -2326,7 +2323,7 @@
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="J4" s="19"/>
     </row>
@@ -2349,10 +2346,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2496,7 +2493,7 @@
       <c r="H6" s="29"/>
       <c r="I6" s="30"/>
     </row>
-    <row r="7" spans="1:9" ht="94.5">
+    <row r="7" spans="1:9" ht="63">
       <c r="A7" s="29">
         <v>3</v>
       </c>
@@ -2504,14 +2501,14 @@
         <v>72</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29" t="s">
         <v>143</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>70</v>
@@ -2519,7 +2516,7 @@
       <c r="H7" s="29"/>
       <c r="I7" s="30"/>
     </row>
-    <row r="8" spans="1:9" ht="63">
+    <row r="8" spans="1:9" ht="78.75">
       <c r="A8" s="29">
         <v>4</v>
       </c>
@@ -2527,14 +2524,14 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29" t="s">
         <v>143</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>70</v>
@@ -2542,7 +2539,7 @@
       <c r="H8" s="29"/>
       <c r="I8" s="30"/>
     </row>
-    <row r="9" spans="1:9" ht="78.75">
+    <row r="9" spans="1:9" ht="31.5">
       <c r="A9" s="29">
         <v>5</v>
       </c>
@@ -2550,14 +2547,14 @@
         <v>74</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29" t="s">
         <v>143</v>
       </c>
       <c r="F9" s="29" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="G9" s="29" t="s">
         <v>70</v>
@@ -2565,7 +2562,7 @@
       <c r="H9" s="29"/>
       <c r="I9" s="30"/>
     </row>
-    <row r="10" spans="1:9" ht="31.5">
+    <row r="10" spans="1:9" ht="63">
       <c r="A10" s="29">
         <v>6</v>
       </c>
@@ -2573,14 +2570,14 @@
         <v>63</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
         <v>143</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G10" s="29" t="s">
         <v>70</v>
@@ -2588,7 +2585,7 @@
       <c r="H10" s="29"/>
       <c r="I10" s="30"/>
     </row>
-    <row r="11" spans="1:9" ht="63">
+    <row r="11" spans="1:9" ht="94.5">
       <c r="A11" s="29">
         <v>7</v>
       </c>
@@ -2596,14 +2593,14 @@
         <v>65</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29" t="s">
         <v>143</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G11" s="29" t="s">
         <v>70</v>
@@ -2611,7 +2608,7 @@
       <c r="H11" s="29"/>
       <c r="I11" s="30"/>
     </row>
-    <row r="12" spans="1:9" ht="94.5">
+    <row r="12" spans="1:9" ht="110.25">
       <c r="A12" s="29">
         <v>8</v>
       </c>
@@ -2619,7 +2616,7 @@
         <v>155</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29" t="s">
@@ -2641,23 +2638,23 @@
       <c r="B13" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29" t="s">
+      <c r="C13" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
-    </row>
-    <row r="14" spans="1:9" ht="110.25">
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75">
       <c r="A14" s="29">
         <v>10</v>
       </c>
@@ -2665,22 +2662,20 @@
         <v>159</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>158</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>154</v>
-      </c>
-      <c r="G14" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75">
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:9" ht="110.25">
       <c r="A15" s="29">
         <v>11</v>
       </c>
@@ -2688,20 +2683,18 @@
         <v>162</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
-      <c r="F15" s="28" t="s">
-        <v>161</v>
-      </c>
+      <c r="F15" s="28"/>
       <c r="G15" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H15" s="28"/>
       <c r="I15" s="28"/>
     </row>
-    <row r="16" spans="1:9" ht="110.25">
+    <row r="16" spans="1:9" ht="78.75">
       <c r="A16" s="29">
         <v>12</v>
       </c>
@@ -2709,58 +2702,48 @@
         <v>163</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>119</v>
+        <v>165</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
+      <c r="F16" s="28" t="s">
+        <v>161</v>
+      </c>
       <c r="G16" s="28" t="s">
         <v>70</v>
       </c>
       <c r="H16" s="28"/>
       <c r="I16" s="28"/>
     </row>
-    <row r="17" spans="1:9" ht="78.75">
-      <c r="A17" s="29">
-        <v>13</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>167</v>
-      </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
+    <row r="17" spans="1:9" ht="15.75">
+      <c r="A17" s="14"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" ht="15.75">
-      <c r="A18" s="14"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
+      <c r="A18" s="17"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
     </row>
     <row r="19" spans="1:9" ht="15.75">
-      <c r="A19" s="17"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
     </row>
     <row r="20" spans="1:9" ht="15.75">
       <c r="C20" s="32"/>
@@ -2788,15 +2771,6 @@
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
       <c r="I22" s="32"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75">
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2817,8 +2791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2964,7 +2938,7 @@
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
       <c r="K5" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L5" s="22"/>
     </row>
@@ -3012,7 +2986,7 @@
       <c r="I7" s="22"/>
       <c r="J7" s="22"/>
       <c r="K7" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L7" s="22"/>
     </row>
@@ -3036,7 +3010,7 @@
       <c r="I8" s="22"/>
       <c r="J8" s="22"/>
       <c r="K8" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L8" s="22"/>
     </row>
@@ -3060,7 +3034,7 @@
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L9" s="22"/>
     </row>
@@ -3084,7 +3058,7 @@
       <c r="I10" s="22"/>
       <c r="J10" s="22"/>
       <c r="K10" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L10" s="22"/>
     </row>
@@ -3108,7 +3082,7 @@
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L11" s="22"/>
     </row>
@@ -3132,7 +3106,7 @@
       <c r="I12" s="22"/>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L12" s="22"/>
     </row>
@@ -3156,7 +3130,7 @@
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L13" s="22"/>
     </row>
@@ -3236,6 +3210,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="H1:H2"/>
@@ -3244,16 +3228,6 @@
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>